<commit_message>
BDD_Naveen Labs_Code Data push
</commit_message>
<xml_diff>
--- a/src/main/resources/data/TestData1.xlsx
+++ b/src/main/resources/data/TestData1.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramad\IdeaProjects\Quantum_NaveenLabs_bdd\src\main\resources\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramad\IdeaProjects\Assignment-NaveenLabs\src\main\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9CE91C-970D-4E4C-B72C-498BC71A1A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{E7EFACAB-82E1-4AAE-9E23-935E3744CCE1}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D4D4D9D6-D460-42E4-B8AD-ED4A3F6A61E5}"/>
+    <workbookView activeTab="1" windowHeight="12456" windowWidth="23256" xWindow="-108" xr2:uid="{D4D4D9D6-D460-42E4-B8AD-ED4A3F6A61E5}" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="UserList" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
+    <sheet name="UserList" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="58">
   <si>
     <t>TestID</t>
   </si>
@@ -201,12 +201,22 @@
   </si>
   <si>
     <t>Test19</t>
+  </si>
+  <si>
+    <t>TestUSer2@gmail.com</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>YES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -262,21 +272,21 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -293,10 +303,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -331,7 +341,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -383,7 +393,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -494,21 +504,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -525,7 +535,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -577,27 +587,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F51A20E-C03A-4B74-AA06-8DECB01B9C73}">
-  <dimension ref="A1:G10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F51A20E-C03A-4B74-AA06-8DECB01B9C73}">
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.77734375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.77734375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="19.77734375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -833,27 +843,27 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{7D1BD035-740E-489F-9C1D-8B462CF8A4C3}"/>
-    <hyperlink ref="F3" r:id="rId2" xr:uid="{13522667-F246-4D4E-B2BD-FCBE2492114A}"/>
-    <hyperlink ref="F4:F10" r:id="rId3" display="TestUSer1@gmail.com" xr:uid="{7864750E-18F4-4292-B289-C812DA31BA7F}"/>
+    <hyperlink r:id="rId1" ref="F2" xr:uid="{7D1BD035-740E-489F-9C1D-8B462CF8A4C3}"/>
+    <hyperlink r:id="rId2" ref="F3" xr:uid="{13522667-F246-4D4E-B2BD-FCBE2492114A}"/>
+    <hyperlink display="TestUSer1@gmail.com" r:id="rId3" ref="F4:F10" xr:uid="{7864750E-18F4-4292-B289-C812DA31BA7F}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D2415F-C86A-477D-BE21-B3075AEBDF5E}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59D2415F-C86A-477D-BE21-B3075AEBDF5E}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" customWidth="1"/>
-    <col min="2" max="3" width="25.21875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="9.77734375" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" width="25.21875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -880,6 +890,9 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -891,24 +904,30 @@
       <c r="C3" t="s">
         <v>8</v>
       </c>
+      <c r="D3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s">
         <v>20</v>
       </c>
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{F7F949F2-540E-45D9-809E-9448159ABDC1}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{B04ED3CB-A43B-4292-8F21-D420D755B859}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{C7F1B130-70CA-4712-961B-8D882DB5EC05}"/>
+    <hyperlink r:id="rId1" ref="B2" xr:uid="{F7F949F2-540E-45D9-809E-9448159ABDC1}"/>
+    <hyperlink r:id="rId2" ref="B3" xr:uid="{B04ED3CB-A43B-4292-8F21-D420D755B859}"/>
+    <hyperlink r:id="rId3" ref="B4" xr:uid="{C7F1B130-70CA-4712-961B-8D882DB5EC05}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>